<commit_message>
Update the contacts in Contractors.xlsx
</commit_message>
<xml_diff>
--- a/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
+++ b/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
@@ -482,12 +482,16 @@
   </si>
   <si>
     <t>10/6: Contacted. VM. Sent a text.
-10/16: After other attempts to make contact I learned that I had an old phone number. Raj called and handed Merrick the phone.10/19: Established contact by phone. Sent plans and arranged site visit for Wednesday 10/21 10am.</t>
+10/16: After other attempts to make contact I learned that I had an old phone number. Raj called and handed Merrick the phone.10/19: Established contact by phone. Sent plans and arranged site visit for Wednesday 10/21 10am.
+10/21: Site visit went ok. I believe we agreed he would send an estimate.
+11/6: Haven't heard from Merrick since the site visit. Asked for an estimate.</t>
   </si>
   <si>
     <t>10/6: Established contact by phone and email. Arranged site visit for Friday
 10/16 afternoon.
-10/16: Site visit went well. I loaned Martin the drawings. He will return on Monday. He warned that we will have to pay for a bigger line from the street to the house for 4.5 baths. He is working on a bid.</t>
+10/16: Site visit went well. I loaned Martin the drawings. He will return on Monday. He warned that we will have to pay for a bigger line from the street to the house for 4.5 baths. He is working on a bid.
+10/21: Drawings returned.
+11/6: I haven't heard from Martin. I emailed him asking for an estimate, including a seasonal maintenance visit and the cost and impact (stone retaining wall and walk) related to a new 3-inch service line.</t>
   </si>
 </sst>
 </file>
@@ -1358,10 +1362,10 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1522,7 +1526,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>126</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
Touching base with electrician
</commit_message>
<xml_diff>
--- a/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
+++ b/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
@@ -481,17 +481,18 @@
     <t>m: 301-793-3127</t>
   </si>
   <si>
-    <t>10/6: Contacted. VM. Sent a text.
-10/16: After other attempts to make contact I learned that I had an old phone number. Raj called and handed Merrick the phone.10/19: Established contact by phone. Sent plans and arranged site visit for Wednesday 10/21 10am.
-10/21: Site visit went ok. I believe we agreed he would send an estimate.
-11/6: Haven't heard from Merrick since the site visit. Asked for an estimate.</t>
-  </si>
-  <si>
     <t>10/6: Established contact by phone and email. Arranged site visit for Friday
 10/16 afternoon.
 10/16: Site visit went well. I loaned Martin the drawings. He will return on Monday. He warned that we will have to pay for a bigger line from the street to the house for 4.5 baths. He is working on a bid.
 10/21: Drawings returned.
 11/6: I haven't heard from Martin. I emailed him asking for an estimate, including a seasonal maintenance visit and the cost and impact (stone retaining wall and walk) related to a new 3-inch service line.</t>
+  </si>
+  <si>
+    <t>10/6: Contacted. VM. Sent a text.
+10/16: After other attempts to make contact I learned that I had an old phone number. Raj called and handed Merrick the phone.10/19: Established contact by phone. Sent plans and arranged site visit for Wednesday 10/21 10am.
+10/21: Site visit went ok. I believe we agreed he would send an estimate.
+11/6: Haven't heard from Merrick since the site visit. Asked for an estimate.
+11/11: Sent another ping asking for the estimate. Merrick responded same day saying he would send estimate to me by the end of the week.</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1366,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,13 +1547,13 @@
         <v>131</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>140</v>
       </c>
@@ -1572,7 +1573,7 @@
         <v>144</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Add documents from OMF Move drafts of contract and scope of work
</commit_message>
<xml_diff>
--- a/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
+++ b/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="212">
   <si>
     <t>Apergis</t>
   </si>
@@ -615,12 +615,6 @@
     <t>R&amp;B Incorporated</t>
   </si>
   <si>
-    <t>sales@rbincorporated.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w: 703-683-1996 </t>
-  </si>
-  <si>
     <t>w: 301-937-8292</t>
   </si>
   <si>
@@ -703,6 +697,27 @@
     <t>12/9: Called. Priced the disconnect of 2 AC units at $500. Arranged the job for Friday at 10am. We will discuss rest of project.
 12/10: Shawn Mullan called asked if he could come early, 9am.
 12/11: Shawn arrived 10 minutes early and completed disconnect in 1 hour. Started to discuss rest of project and he said I should talk to his father-in-law Bob, furnace expert. Sent drawings and rfp.</t>
+  </si>
+  <si>
+    <t>Snyder</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>w: 703-683-1996 
+m: 571-238-9099</t>
+  </si>
+  <si>
+    <t>sales@rbincorporated.com
+dave@rbincorporated.com</t>
+  </si>
+  <si>
+    <t>A/C &amp; Heating
+Sheet Metal
+UNICO
+Parts
+Duct Cleaning</t>
   </si>
 </sst>
 </file>
@@ -1614,10 +1629,10 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,21 +1833,21 @@
         <v>175</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>160</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>153</v>
@@ -1847,13 +1862,13 @@
         <v>156</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>162</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1876,7 +1891,7 @@
         <v>174</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>176</v>
@@ -1894,62 +1909,68 @@
         <v>178</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="C11" s="5" t="s">
         <v>182</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>119</v>
+        <v>211</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>183</v>
+        <v>210</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>101</v>
@@ -1967,7 +1988,7 @@
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G13" s="13"/>
     </row>
@@ -2009,13 +2030,13 @@
         <v>152</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>163</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2038,7 +2059,7 @@
         <v>167</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>161</v>
@@ -2083,7 +2104,7 @@
     <hyperlink ref="E7" r:id="rId9"/>
     <hyperlink ref="E16" r:id="rId10"/>
     <hyperlink ref="E9" r:id="rId11"/>
-    <hyperlink ref="E11" r:id="rId12"/>
+    <hyperlink ref="E11" r:id="rId12" display="sales@rbincorporated.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId13"/>

</xml_diff>

<commit_message>
Final changes to achieve ScopeOfWork-Final-2.pdf Archive Contractor schedule of values, construction schedule, insurance etc.
</commit_message>
<xml_diff>
--- a/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
+++ b/house/20140216 Porch and Master Bath/Contractors/Contractors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GC" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="215">
   <si>
     <t>Apergis</t>
   </si>
@@ -531,9 +531,6 @@
     <t>info@aspenhillplumbing.com</t>
   </si>
   <si>
-    <t>w: 301-933-0801</t>
-  </si>
-  <si>
     <t>Stevens Co.</t>
   </si>
   <si>
@@ -665,15 +662,6 @@
 12/7: Called. Declined. Too busy.</t>
   </si>
   <si>
-    <t>12/5:  Called late, no answer. Sent email describing project and including plans. Invited for a visit.
-12/7: Called. Receptionist took my name and contact. Rob called me back. We made an appointment for Thursday Dec 10 at 8am</t>
-  </si>
-  <si>
-    <t>12/5: Called late, no answer. Sent email describing project and including plans. Invited for a visit and to submit a bid.
-12/7: Dave Glick (owner) responded. Offered to come Monday 2-4pm or Tuesday 7-8am. I accepted Monday 2pm.
-12/8: Dave confirmed. He will call with 30 min ETA.</t>
-  </si>
-  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -688,15 +676,6 @@
   <si>
     <t>600 Gallatin St NW
 Washington DC 20011</t>
-  </si>
-  <si>
-    <t>w: 202-291-1000
-m: 410-963-5365</t>
-  </si>
-  <si>
-    <t>12/9: Called. Priced the disconnect of 2 AC units at $500. Arranged the job for Friday at 10am. We will discuss rest of project.
-12/10: Shawn Mullan called asked if he could come early, 9am.
-12/11: Shawn arrived 10 minutes early and completed disconnect in 1 hour. Started to discuss rest of project and he said I should talk to his father-in-law Bob, furnace expert. Sent drawings and rfp.</t>
   </si>
   <si>
     <t>Snyder</t>
@@ -718,6 +697,39 @@
 UNICO
 Parts
 Duct Cleaning</t>
+  </si>
+  <si>
+    <t>12/5:  Called late, no answer. Sent email describing project and including plans. Invited for a visit.
+12/7: Called. Receptionist took my name and contact. Rob called me back. We made an appointment for Thursday Dec 10 at 8am
+12/10: Site visit went well. Talked a good game. Will send an estimate.</t>
+  </si>
+  <si>
+    <t>Mullan</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>m: 410-963-5365</t>
+  </si>
+  <si>
+    <t>w: 202-291-1000</t>
+  </si>
+  <si>
+    <t>w: 301-933-0801
+m: 240-644-4673</t>
+  </si>
+  <si>
+    <t>12/9: Called. Priced the disconnect of 2 AC units at $500. Arranged the job for Friday at 10am. We will discuss rest of project.
+12/10: Shawn Mullan called asked if he could come early, 9am.
+12/11: Shawn arrived 10 minutes early and completed disconnect in 1 hour. Started to discuss rest of project and he said I should talk to his father-in-law Bob, furnace expert. Sent drawings and rfp.
+12/15: Had not heard anything. Called to see if interested. Agreed on site visit on Wed 12/16 around 4pm. Need to deal with drain in foundation.</t>
+  </si>
+  <si>
+    <t>12/5: Called late, no answer. Sent email describing project and including plans. Invited for a visit and to submit a bid.
+12/7: Dave Glick (owner) responded. Offered to come Monday 2-4pm or Tuesday 7-8am. I accepted Monday 2pm.
+12/8: Dave confirmed. He will call with 30 min ETA.
+12/14: Site visit went well. Suggested keep the stack outside to the existing (to be moved) drain. Same with drain for utility sink. Also suggested to keep heating system simple. Will send estimate by the end of the week. Does not believe can do the work before the new year.</t>
   </si>
 </sst>
 </file>
@@ -741,7 +753,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -757,12 +769,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -831,9 +837,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1626,13 +1629,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,7 +1734,7 @@
       <c r="F3" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>122</v>
       </c>
       <c r="H3" s="5" t="s">
@@ -1786,7 +1789,7 @@
       <c r="F5" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>123</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -1821,33 +1824,33 @@
     </row>
     <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>160</v>
-      </c>
       <c r="I7" s="5" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="255" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>184</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>185</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>153</v>
@@ -1859,118 +1862,116 @@
         <v>155</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="G9" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>119</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H10" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="240" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="180" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>203</v>
-      </c>
+      <c r="E12" s="7"/>
       <c r="F12" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>206</v>
+        <v>211</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>213</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>101</v>
@@ -1978,116 +1979,137 @@
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" ht="270" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="E14" s="7"/>
+      <c r="F14" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B15" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
-        <v>151</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>144</v>
+      </c>
       <c r="F15" s="5" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>165</v>
-      </c>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="C16" s="5" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>168</v>
-      </c>
+      <c r="E16" s="7"/>
       <c r="F16" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G16" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>187</v>
       </c>
+      <c r="H16" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="I16" s="5" t="s">
-        <v>161</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E18" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F18" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H18" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2098,11 +2120,11 @@
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
     <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E17" r:id="rId6"/>
-    <hyperlink ref="E14" r:id="rId7" display="merrickbes@gmail.com"/>
+    <hyperlink ref="E18" r:id="rId6"/>
+    <hyperlink ref="E15" r:id="rId7" display="merrickbes@gmail.com"/>
     <hyperlink ref="E8" r:id="rId8"/>
     <hyperlink ref="E7" r:id="rId9"/>
-    <hyperlink ref="E16" r:id="rId10"/>
+    <hyperlink ref="E17" r:id="rId10"/>
     <hyperlink ref="E9" r:id="rId11"/>
     <hyperlink ref="E11" r:id="rId12" display="sales@rbincorporated.com"/>
   </hyperlinks>

</xml_diff>